<commit_message>
feat: add create custom sheet
</commit_message>
<xml_diff>
--- a/build/resources/main/planilha_financeira.xlsx
+++ b/build/resources/main/planilha_financeira.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kacia\Documents\wcc-kotlin-telegram-bot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831FEE3F-23C1-4D98-8280-AEC40C601358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6F9DDD-9C5B-4119-BF12-E9B4BD052AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDDF05E2-581B-48F9-AC5E-756D300973F6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Financeiro" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>